<commit_message>
works but no colors yet
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Root\Dev\Python_projects\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Root\Dev\Python_projects\spreadsheet_compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD83D75-876C-4A79-A4F3-660FB74E9846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C125A0-AF97-472B-8374-FD8E8095E173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>